<commit_message>
docs: add mid-report and update documents
</commit_message>
<xml_diff>
--- a/2.WBS/xlsx/WBS_현대이지웰_최종프로젝트.xlsx
+++ b/2.WBS/xlsx/WBS_현대이지웰_최종프로젝트.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GamesungCoding\ResourceRepo\2.WBS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GamesungCoding\ResourceRepo\2.WBS\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7F2796-9D0E-4DF0-96BB-6D0452D56202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93F8EBD-CABE-466A-9AE6-B6609EA792D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -921,6 +921,15 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,15 +937,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1199,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2986,7 +2986,7 @@
       </c>
       <c r="C19" s="37">
         <f>IF(COUNTBLANK(C20:C21)=2, "", SUM(C20:C21)/COUNT(C20:C21))</f>
-        <v>0.01</v>
+        <v>0.41500000000000004</v>
       </c>
       <c r="D19" s="10">
         <f>IF(AND(F19&lt;&gt;"", E19&lt;&gt;""), F19-E19+1, "")</f>
@@ -3071,7 +3071,7 @@
         <v>36</v>
       </c>
       <c r="C20" s="37">
-        <v>0.02</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D20" s="10">
         <v>31</v>
@@ -3154,7 +3154,7 @@
         <v>37</v>
       </c>
       <c r="C21" s="37">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D21" s="10">
         <v>31</v>
@@ -8225,22 +8225,22 @@
       <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="55"/>
-      <c r="B2" s="69"/>
+      <c r="B2" s="66"/>
       <c r="C2" s="34" t="s">
         <v>44</v>
       </c>
@@ -8330,13 +8330,13 @@
       <c r="B7" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="67"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="70"/>
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="50"/>
@@ -8409,13 +8409,13 @@
       <c r="B12" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="65"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="67"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="70"/>
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="50"/>
@@ -8505,13 +8505,13 @@
       <c r="B18" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="67"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="70"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="50"/>
@@ -8548,13 +8548,13 @@
       <c r="B21" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="65"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="67"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="70"/>
     </row>
     <row r="22" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="50"/>
@@ -8591,13 +8591,13 @@
       <c r="B24" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="67"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="70"/>
     </row>
     <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="50"/>
@@ -8634,13 +8634,13 @@
       <c r="B27" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="65"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="70"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="50"/>
@@ -8677,13 +8677,13 @@
       <c r="B30" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="67"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="70"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="50"/>
@@ -8717,11 +8717,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="C7:I7"/>
     <mergeCell ref="C24:I24"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="C12:I12"/>
@@ -8729,6 +8724,11 @@
     <mergeCell ref="A7:A32"/>
     <mergeCell ref="C27:I27"/>
     <mergeCell ref="C30:I30"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>